<commit_message>
added a few options
</commit_message>
<xml_diff>
--- a/BadEvents (Repaired).xlsx
+++ b/BadEvents (Repaired).xlsx
@@ -5,7 +5,7 @@
   <workbookPr checkCompatibility="1" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\unitything\Be-a-god\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\banner.main.ad.rit.edu\students\rwg6766\IGMProfile\Documents\Github\Be-a-god\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="93">
   <si>
     <t>Event</t>
   </si>
@@ -148,12 +148,6 @@
     <t>Neighboring nation is attacking???</t>
   </si>
   <si>
-    <t>Using your brush of magnificance, you paint the sky with a adjective rainbow. Your people are amused.</t>
-  </si>
-  <si>
-    <t>Your people are bored , one of them is kicking a tumble weed.</t>
-  </si>
-  <si>
     <t>Oracle vision.</t>
   </si>
   <si>
@@ -235,9 +229,6 @@
     <t xml:space="preserve">Without much effort, you dip your fingers in your chalice and lightly sprinkle the sparse land below. The people are happy that rain has come their way. Some feel that this is a good sign and are gambling more </t>
   </si>
   <si>
-    <t>An earthquake shakes the ground, some of your follower's buildings and houses are destroyed.</t>
-  </si>
-  <si>
     <t>A snowstorm approaches. Weather reports have estimated a foot of snow.</t>
   </si>
   <si>
@@ -275,6 +266,45 @@
   </si>
   <si>
     <t>With little effort, you apply force using a single finger to counter act the quake. The quake shivers in fear to your touch and disspates instantly. Your people are as equally amazed as you are.</t>
+  </si>
+  <si>
+    <t>In a fit of anger, you rain fire down upon the villagers! Are they not entertained?</t>
+  </si>
+  <si>
+    <t>Nothing incredible has happened lately. Your people are bored and complaining, one of them is kicking a tumble weed.</t>
+  </si>
+  <si>
+    <t>Using your brush of magnificance, you paint the sky with a marvelous rainbow. Your people are amused.</t>
+  </si>
+  <si>
+    <t>You strike down one of your followers with a brilliant flash of lightning. They certainly aren't bored anymore.</t>
+  </si>
+  <si>
+    <t>In an act of generosity, you drip water from your chalice upon the village crops. The villagers rejoice in their harvest.</t>
+  </si>
+  <si>
+    <t>You give the little heretic a plague of severe itchyness. He seems to have learned his lesson, and now everyday he does extra Holy Jumping Jacks.</t>
+  </si>
+  <si>
+    <t>In your rage you hurled down a mighty thunderbolt to smite the sinful rebel, but you missed and hit the cheese-maker. The movement doubles in strength.</t>
+  </si>
+  <si>
+    <t>You struck down the sinful rebel with a blinding flash of lightning.None of your follows skipped their Holy Jumping Jacks that day.</t>
+  </si>
+  <si>
+    <t>You plagued the little heretic with relentless sneezing. He seems to have become angry and the movement continues.</t>
+  </si>
+  <si>
+    <t>You beset the nay-sayer with nightmares and visions of inconceivable horror. Nothing has changed, he must have forgot his dreams.</t>
+  </si>
+  <si>
+    <t>You appear before the nay-sayer in a dream in all your glory… then smack him across the face. The next day he hastily ended the movement.</t>
+  </si>
+  <si>
+    <t>You reach to the sun and scoop a mighty fire-ball then drop it upon the rebelious movement. Many people died, but most of them were rebels… you know… probably.</t>
+  </si>
+  <si>
+    <t>You unleash a vicious plague of mosquitos upon your people until they repent their sinful ways. The nay-sayer quickly loses all his support.</t>
   </si>
 </sst>
 </file>
@@ -597,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,13 +701,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -731,45 +761,54 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>82</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -782,54 +821,54 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="G28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="G29" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>21</v>
@@ -837,85 +876,109 @@
     </row>
     <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="H30" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B38" s="1" t="s">
+      <c r="D38" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="F38" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>